<commit_message>
240509 - 수정 완
</commit_message>
<xml_diff>
--- a/doc/WCS 알고리즘 평가 기준.xlsx
+++ b/doc/WCS 알고리즘 평가 기준.xlsx
@@ -9,11 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="특성, 평가 기준 예시" sheetId="1" r:id="rId1"/>
-    <sheet name="동작 Sheet 예시" sheetId="3" r:id="rId2"/>
+    <sheet name="초기 조건" sheetId="1" r:id="rId1"/>
+    <sheet name="동작 리스트" sheetId="6" r:id="rId2"/>
+    <sheet name="입력 데이터 예시" sheetId="5" r:id="rId3"/>
+    <sheet name="동작 Sheet 예시" sheetId="3" r:id="rId4"/>
+    <sheet name="평가 기준" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,11 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="99">
-  <si>
-    <t>평가 조건</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="102">
   <si>
     <t>IN 빈도</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -148,10 +147,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>시간 (단위 시간) (70%)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>정렬 전 
 대기 시간</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -180,10 +175,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>미션 리스트</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>동작</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -263,10 +254,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>YYMMDD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>동작 리스트</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -359,27 +346,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>통신(계산 수)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>갠트리 이동 속도 (1U/1t)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Z축 높이(낮을 수록 좋음)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>평균 높이 / 
-(표준 편차 * 최대 높이)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>정렬 (마지막 배치 기준) (30%)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>WAIT 명령 직후 WAIT 명령 배치 금지</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -389,16 +355,6 @@
   </si>
   <si>
     <t>β&gt;60</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DB 데이터 요청/수정 횟수 n
-* α(현재0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>(XY평면 이동시간)
-+ Z축 이동시간</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -428,6 +384,78 @@
   <si>
     <t>기본 제품 
 I/O 전략</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>평가 조건</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1 - (알고리즘시간/기준시간)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>알고리즘 시간 = (XY 수평 이동 시간) + Z 축 이동 시간</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1 / 최상단 상품 평균 높이</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>YYYYMMDD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>미션 리스트 (SEED = 12345)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>필요시</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이후</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>반복</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정렬 (마지막 배치 기준) 
+(30%)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>갠트리 총 이동 시간 (WAIT 명령 제외)
+(단위 시간 U) (70%)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,7 +466,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -506,6 +534,14 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -527,7 +563,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="56">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -760,17 +796,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -884,17 +909,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -990,15 +1004,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -1216,13 +1221,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1283,10 +1314,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1">
@@ -1313,12 +1344,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1337,19 +1362,19 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1358,260 +1383,182 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="49" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="50" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1619,31 +1566,61 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1926,9 +1903,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R25"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1942,593 +1921,176 @@
     <col min="22" max="22" width="9.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:18" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="80" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="82"/>
-      <c r="H2" s="80" t="s">
+    <row r="1" spans="1:13" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:13" ht="50.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="58"/>
+    </row>
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="59" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="61"/>
+      <c r="E3" s="63" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
-      <c r="N2" s="81"/>
-      <c r="O2" s="81"/>
-      <c r="P2" s="81"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="49" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="83" t="s">
+    </row>
+    <row r="4" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="60"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="62"/>
+    </row>
+    <row r="5" spans="1:13" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="36" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="83" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="85"/>
-      <c r="E3" s="87" t="s">
-        <v>98</v>
-      </c>
-      <c r="F3" s="85" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="89" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="91"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="95" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="90"/>
-      <c r="P3" s="90"/>
-      <c r="Q3" s="91"/>
-      <c r="R3" s="97" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="86"/>
-      <c r="E4" s="88"/>
-      <c r="F4" s="86"/>
-      <c r="H4" s="92"/>
-      <c r="I4" s="93"/>
-      <c r="J4" s="93"/>
-      <c r="K4" s="93"/>
-      <c r="L4" s="94"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="93"/>
-      <c r="P4" s="93"/>
-      <c r="Q4" s="94"/>
-      <c r="R4" s="98"/>
-    </row>
-    <row r="5" spans="1:18" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="38" t="s">
+      <c r="E5" s="40"/>
+      <c r="F5" s="38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="36">
+        <v>1</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="D6" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="H5" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="I5" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="K5" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="L5" s="26" t="s">
-        <v>3</v>
-      </c>
-      <c r="M5" s="5"/>
-      <c r="N5" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="O5" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="P5" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="R5" s="20"/>
-    </row>
-    <row r="6" spans="1:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="38">
-        <v>1</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="F6" s="40">
+      <c r="E6" s="40" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="38">
         <v>60</v>
       </c>
-      <c r="H6" s="32">
-        <v>1</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="K6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="4">
-        <v>1</v>
-      </c>
-      <c r="O6" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q6" s="28" t="s">
+    </row>
+    <row r="7" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="69" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="71" t="s">
         <v>92</v>
       </c>
-      <c r="R6" s="21" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="70" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="72" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="74" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" s="76"/>
-      <c r="F7" s="78"/>
-      <c r="H7" s="32">
-        <v>2</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="K7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="5"/>
-      <c r="N7" s="4">
-        <v>2</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="P7" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="71"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="77"/>
-      <c r="F8" s="79"/>
-      <c r="H8" s="32">
-        <v>3</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="K8" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="21" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="135" t="s">
-        <v>94</v>
+      <c r="F7" s="73"/>
+    </row>
+    <row r="8" spans="1:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="66"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="72"/>
+      <c r="F8" s="74"/>
+    </row>
+    <row r="9" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>83</v>
       </c>
       <c r="B9" s="4">
-        <v>3</v>
-      </c>
-      <c r="C9" s="138">
+        <v>20</v>
+      </c>
+      <c r="C9" s="51">
         <v>-1</v>
       </c>
-      <c r="D9" s="43">
+      <c r="D9" s="41">
         <f>B9+1</f>
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="E9" s="17"/>
       <c r="F9" s="18"/>
-      <c r="H9" s="37">
-        <v>4</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="19"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="4">
-        <v>6</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P9" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q9" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="R9" s="21" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="136" t="s">
-        <v>95</v>
+    </row>
+    <row r="10" spans="1:13" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="49" t="s">
+        <v>84</v>
       </c>
       <c r="B10" s="4">
-        <v>3</v>
-      </c>
-      <c r="C10" s="139">
+        <v>20</v>
+      </c>
+      <c r="C10" s="52">
         <v>-1</v>
       </c>
-      <c r="D10" s="43">
-        <f t="shared" ref="D10:D11" si="0">B10+1</f>
-        <v>4</v>
+      <c r="D10" s="41">
+        <f>B10+1</f>
+        <v>21</v>
       </c>
       <c r="E10" s="17"/>
       <c r="F10" s="18"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="4">
-        <v>7</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="R10" s="21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="137" t="s">
-        <v>96</v>
+    </row>
+    <row r="11" spans="1:13" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="50" t="s">
+        <v>85</v>
       </c>
       <c r="B11" s="13">
-        <v>4</v>
-      </c>
-      <c r="C11" s="140">
+        <v>5</v>
+      </c>
+      <c r="C11" s="53">
         <v>0</v>
       </c>
-      <c r="D11" s="44">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E11" s="45"/>
-      <c r="F11" s="46"/>
-      <c r="H11" s="111" t="s">
-        <v>35</v>
-      </c>
-      <c r="I11" s="112"/>
-      <c r="J11" s="112"/>
-      <c r="K11" s="112"/>
-      <c r="L11" s="112"/>
-      <c r="M11" s="5"/>
-      <c r="N11" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" ht="34.5" x14ac:dyDescent="0.3">
-      <c r="H12" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="J12" s="24" t="s">
+      <c r="D11" s="42">
+        <v>0</v>
+      </c>
+      <c r="E11" s="43"/>
+      <c r="F11" s="44"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>12</v>
-      </c>
-      <c r="M12" s="5"/>
-      <c r="N12" s="4">
-        <v>100</v>
-      </c>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="R12" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="21" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H13" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" s="68"/>
-      <c r="J13" s="68"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="8"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="15"/>
-    </row>
-    <row r="14" spans="1:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="15" spans="1:18" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="99" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="100"/>
-      <c r="D15" s="100"/>
-      <c r="E15" s="101"/>
-      <c r="N15" s="59" t="s">
-        <v>60</v>
-      </c>
-      <c r="O15" s="60"/>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="60"/>
-      <c r="R15" s="61"/>
-    </row>
-    <row r="16" spans="1:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="102" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="103"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="104"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="65" t="s">
-        <v>39</v>
-      </c>
-      <c r="O16" s="62" t="s">
-        <v>68</v>
-      </c>
-      <c r="P16" s="63"/>
-      <c r="Q16" s="64"/>
-      <c r="R16" s="57" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="2:18" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="105"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="107"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="66"/>
-      <c r="O17" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="P17" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q17" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="R17" s="58"/>
-    </row>
-    <row r="18" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="108" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="109"/>
-      <c r="D18" s="109" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" s="110"/>
-      <c r="M18" s="48"/>
-      <c r="N18" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="O18" s="54" t="s">
-        <v>67</v>
-      </c>
-      <c r="P18" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q18" s="36"/>
-      <c r="R18" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B19" s="118" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="119"/>
-      <c r="D19" s="122" t="s">
-        <v>90</v>
-      </c>
-      <c r="E19" s="123"/>
-      <c r="M19" s="48"/>
-      <c r="N19" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="O19" s="55"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="36"/>
-      <c r="R19" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="120"/>
-      <c r="C20" s="121"/>
-      <c r="D20" s="124"/>
-      <c r="E20" s="125"/>
-      <c r="M20" s="48"/>
-      <c r="N20" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="R20" s="19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B21" s="113" t="s">
-        <v>86</v>
-      </c>
-      <c r="C21" s="114"/>
-      <c r="D21" s="114"/>
-      <c r="E21" s="115"/>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B22" s="105"/>
-      <c r="C22" s="106"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="107"/>
-    </row>
-    <row r="23" spans="2:18" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="B23" s="116" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="117"/>
-      <c r="D23" s="30"/>
-      <c r="E23" s="31"/>
-    </row>
-    <row r="24" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="126" t="s">
-        <v>85</v>
-      </c>
-      <c r="C24" s="127"/>
-      <c r="D24" s="50"/>
-      <c r="E24" s="51"/>
-    </row>
-    <row r="25" spans="2:18" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B25" s="128"/>
-      <c r="C25" s="129"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
-    </row>
+    </row>
+    <row r="16" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M16" s="55"/>
+    </row>
+    <row r="17" spans="13:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M17" s="55"/>
+    </row>
+    <row r="18" spans="13:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="M18" s="46"/>
+    </row>
+    <row r="19" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M19" s="46"/>
+    </row>
+    <row r="20" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M20" s="46"/>
+    </row>
+    <row r="24" spans="13:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B19:C20"/>
-    <mergeCell ref="D19:E20"/>
-    <mergeCell ref="B24:C25"/>
-    <mergeCell ref="B16:E17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="B21:E22"/>
-    <mergeCell ref="H3:L4"/>
-    <mergeCell ref="N3:Q4"/>
-    <mergeCell ref="R3:R4"/>
-    <mergeCell ref="H2:Q2"/>
-    <mergeCell ref="B15:E15"/>
+  <mergeCells count="11">
+    <mergeCell ref="M16:M17"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:B4"/>
     <mergeCell ref="C3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
-    <mergeCell ref="H13:K13"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:F8"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="R16:R17"/>
-    <mergeCell ref="N15:R15"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="N16:N17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2538,10 +2100,438 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G102"/>
+  <dimension ref="B1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D101" sqref="D101"/>
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="5" width="17.875" customWidth="1"/>
+    <col min="6" max="6" width="39.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:6" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="B2" s="84" t="s">
+        <v>56</v>
+      </c>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="86"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="82" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="79" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="80"/>
+      <c r="E3" s="81"/>
+      <c r="F3" s="77" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="83"/>
+      <c r="C4" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="78"/>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="75" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="76"/>
+      <c r="D6" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="54" t="s">
+        <v>93</v>
+      </c>
+      <c r="E7" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B2:F2"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:L13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="6" width="15.75" customWidth="1"/>
+    <col min="7" max="7" width="0.625" customWidth="1"/>
+    <col min="8" max="10" width="15.75" customWidth="1"/>
+    <col min="11" max="11" width="26.875" customWidth="1"/>
+    <col min="12" max="12" width="41.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:12" ht="41.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="56" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="47" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="26.25" x14ac:dyDescent="0.3">
+      <c r="B3" s="100" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="88"/>
+      <c r="D3" s="88"/>
+      <c r="E3" s="88"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="87" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="88"/>
+      <c r="J3" s="88"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="93" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B4" s="101"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="92"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="90"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="92"/>
+      <c r="L4" s="94"/>
+    </row>
+    <row r="5" spans="2:12" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="B5" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="J5" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="20"/>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="30">
+        <v>1</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="4">
+        <v>1</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B7" s="30">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="14"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="4">
+        <v>2</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="14"/>
+      <c r="L7" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="30">
+        <v>3</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="35">
+        <v>4</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="19"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="4">
+        <v>6</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="L9" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" ht="33" x14ac:dyDescent="0.3">
+      <c r="B10" s="7"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="4">
+        <v>7</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B11" s="98" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" ht="34.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="4">
+        <v>100</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" ht="21" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="95" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="H3:K4"/>
+    <mergeCell ref="L3:L4"/>
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B3:F4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G103"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2556,32 +2546,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="132" t="s">
-        <v>38</v>
-      </c>
-      <c r="B1" s="133"/>
-      <c r="C1" s="133"/>
-      <c r="D1" s="134"/>
+      <c r="A1" s="104" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="105"/>
+      <c r="C1" s="105"/>
+      <c r="D1" s="106"/>
     </row>
     <row r="2" spans="1:7" ht="38.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="130" t="s">
-        <v>81</v>
-      </c>
-      <c r="D2" s="131"/>
+      <c r="C2" s="102" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="103"/>
       <c r="E2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="F2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -2589,13 +2579,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C3" s="3">
         <v>1</v>
       </c>
       <c r="D3" s="10">
-        <v>2492</v>
+        <v>202492</v>
       </c>
       <c r="E3">
         <f>IF($B3 = "IN", $C3, "")</f>
@@ -2615,7 +2605,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C4" s="3">
         <v>1</v>
@@ -2638,13 +2628,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C5" s="3">
         <v>4</v>
       </c>
       <c r="D5" s="10">
-        <v>23111</v>
+        <v>2023111</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
@@ -2664,13 +2654,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C6" s="3">
         <v>1</v>
       </c>
       <c r="D6" s="10">
-        <v>2438</v>
+        <v>202438</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
@@ -2690,7 +2680,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7" s="3">
         <v>1</v>
@@ -2713,7 +2703,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C8" s="3">
         <v>1345</v>
@@ -2736,13 +2726,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C9" s="3">
         <v>3</v>
       </c>
       <c r="D9" s="10">
-        <v>2224</v>
+        <v>202224</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -2750,7 +2740,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="3">
         <v>1561</v>
@@ -2761,13 +2751,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C11" s="3">
         <v>2</v>
       </c>
       <c r="D11" s="10">
-        <v>24815</v>
+        <v>2024815</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -2775,13 +2765,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
       </c>
       <c r="D12" s="10">
-        <v>22422</v>
+        <v>2022422</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -2789,13 +2779,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C13" s="3">
         <v>3</v>
       </c>
       <c r="D13" s="10">
-        <v>231031</v>
+        <v>20231031</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -2803,13 +2793,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C14" s="3">
         <v>3</v>
       </c>
       <c r="D14" s="10">
-        <v>25222</v>
+        <v>2025222</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -2817,13 +2807,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C15" s="3">
         <v>4</v>
       </c>
       <c r="D15" s="10">
-        <v>25922</v>
+        <v>2025922</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -2831,13 +2821,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C16" s="3">
         <v>2</v>
       </c>
       <c r="D16" s="10">
-        <v>20128</v>
+        <v>2020128</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
@@ -2845,7 +2835,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C17" s="3">
         <v>427</v>
@@ -2856,7 +2846,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C18" s="3">
         <v>4</v>
@@ -2867,7 +2857,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C19" s="3">
         <v>909</v>
@@ -2878,13 +2868,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C20" s="3">
         <v>4</v>
       </c>
       <c r="D20" s="10">
-        <v>22114</v>
+        <v>2022114</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
@@ -2892,13 +2882,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C21" s="3">
         <v>3</v>
       </c>
       <c r="D21" s="10">
-        <v>251114</v>
+        <v>20251114</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -2906,13 +2896,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C22" s="3">
         <v>1</v>
       </c>
       <c r="D22" s="10">
-        <v>2289</v>
+        <v>202289</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
@@ -2920,7 +2910,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C23" s="3">
         <v>2</v>
@@ -2931,7 +2921,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C24" s="3">
         <v>1703</v>
@@ -2942,13 +2932,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C25" s="3">
         <v>4</v>
       </c>
       <c r="D25" s="10">
-        <v>221121</v>
+        <v>20221121</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
@@ -2956,7 +2946,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C26" s="3">
         <v>326</v>
@@ -2967,13 +2957,13 @@
         <v>25</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C27" s="3">
         <v>3</v>
       </c>
       <c r="D27" s="10">
-        <v>21113</v>
+        <v>2021113</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2981,13 +2971,13 @@
         <v>26</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C28" s="3">
         <v>2</v>
       </c>
       <c r="D28" s="10">
-        <v>2197</v>
+        <v>202197</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2995,7 +2985,7 @@
         <v>27</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C29" s="3">
         <v>1</v>
@@ -3006,13 +2996,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C30" s="3">
         <v>3</v>
       </c>
       <c r="D30" s="10">
-        <v>24430</v>
+        <v>2024430</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -3020,13 +3010,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C31" s="3">
         <v>1</v>
       </c>
       <c r="D31" s="10">
-        <v>20721</v>
+        <v>2020721</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -3034,7 +3024,7 @@
         <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C32" s="3">
         <v>972</v>
@@ -3045,13 +3035,13 @@
         <v>31</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C33" s="3">
         <v>2</v>
       </c>
       <c r="D33" s="10">
-        <v>2458</v>
+        <v>202458</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -3059,13 +3049,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C34" s="3">
         <v>2</v>
       </c>
       <c r="D34" s="10">
-        <v>24215</v>
+        <v>2024215</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -3073,7 +3063,7 @@
         <v>33</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C35" s="3">
         <v>1110</v>
@@ -3084,13 +3074,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C36" s="3">
         <v>1</v>
       </c>
       <c r="D36" s="10">
-        <v>25523</v>
+        <v>2025523</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -3098,13 +3088,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C37" s="3">
         <v>3</v>
       </c>
       <c r="D37" s="10">
-        <v>2577</v>
+        <v>202577</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -3112,7 +3102,7 @@
         <v>36</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C38" s="3">
         <v>922</v>
@@ -3123,13 +3113,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C39" s="3">
         <v>1</v>
       </c>
       <c r="D39" s="10">
-        <v>2421</v>
+        <v>202421</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -3137,7 +3127,7 @@
         <v>38</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C40" s="3">
         <v>367</v>
@@ -3148,13 +3138,13 @@
         <v>39</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C41" s="3">
         <v>2</v>
       </c>
       <c r="D41" s="10">
-        <v>25720</v>
+        <v>2025720</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -3162,7 +3152,7 @@
         <v>40</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C42" s="3">
         <v>2</v>
@@ -3173,13 +3163,13 @@
         <v>41</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C43" s="3">
         <v>2</v>
       </c>
       <c r="D43" s="10">
-        <v>211031</v>
+        <v>20211031</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -3187,7 +3177,7 @@
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C44" s="3">
         <v>2</v>
@@ -3198,7 +3188,7 @@
         <v>43</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C45" s="3">
         <v>246</v>
@@ -3209,13 +3199,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C46" s="3">
         <v>1</v>
       </c>
       <c r="D46" s="10">
-        <v>21823</v>
+        <v>2021823</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
@@ -3223,7 +3213,7 @@
         <v>45</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C47" s="3">
         <v>1076</v>
@@ -3234,13 +3224,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C48" s="3">
         <v>3</v>
       </c>
       <c r="D48" s="10">
-        <v>21127</v>
+        <v>2021127</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -3248,7 +3238,7 @@
         <v>47</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C49" s="3">
         <v>1597</v>
@@ -3259,7 +3249,7 @@
         <v>48</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C50" s="3">
         <v>3</v>
@@ -3270,7 +3260,7 @@
         <v>49</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C51" s="3">
         <v>1</v>
@@ -3281,13 +3271,13 @@
         <v>50</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C52" s="3">
         <v>2</v>
       </c>
       <c r="D52" s="10">
-        <v>22923</v>
+        <v>2022923</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
@@ -3295,13 +3285,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C53" s="3">
         <v>3</v>
       </c>
       <c r="D53" s="10">
-        <v>2437</v>
+        <v>202437</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -3309,13 +3299,13 @@
         <v>52</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C54" s="3">
         <v>2</v>
       </c>
       <c r="D54" s="10">
-        <v>2464</v>
+        <v>202464</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -3323,13 +3313,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C55" s="3">
         <v>2</v>
       </c>
       <c r="D55" s="10">
-        <v>251023</v>
+        <v>20251023</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -3337,7 +3327,7 @@
         <v>54</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C56" s="3">
         <v>1</v>
@@ -3348,7 +3338,7 @@
         <v>55</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C57" s="3">
         <v>3</v>
@@ -3359,13 +3349,13 @@
         <v>56</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C58" s="3">
         <v>2</v>
       </c>
       <c r="D58" s="10">
-        <v>2531</v>
+        <v>202531</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -3373,7 +3363,7 @@
         <v>57</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C59" s="3">
         <v>1333</v>
@@ -3384,13 +3374,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C60" s="3">
         <v>2</v>
       </c>
       <c r="D60" s="10">
-        <v>2177</v>
+        <v>202177</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -3398,7 +3388,7 @@
         <v>59</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C61" s="3">
         <v>4</v>
@@ -3409,13 +3399,13 @@
         <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C62" s="3">
         <v>1</v>
       </c>
       <c r="D62" s="10">
-        <v>25921</v>
+        <v>2025921</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -3423,7 +3413,7 @@
         <v>61</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C63" s="3">
         <v>1</v>
@@ -3434,13 +3424,13 @@
         <v>62</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C64" s="3">
         <v>1</v>
       </c>
       <c r="D64" s="10">
-        <v>24130</v>
+        <v>2024130</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -3448,7 +3438,7 @@
         <v>63</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C65" s="3">
         <v>1615</v>
@@ -3459,13 +3449,13 @@
         <v>64</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C66" s="3">
         <v>3</v>
       </c>
       <c r="D66" s="10">
-        <v>21101</v>
+        <v>2021101</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -3473,7 +3463,7 @@
         <v>65</v>
       </c>
       <c r="B67" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C67" s="3">
         <v>1361</v>
@@ -3484,13 +3474,13 @@
         <v>66</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C68" s="3">
         <v>4</v>
       </c>
       <c r="D68" s="10">
-        <v>23131</v>
+        <v>2023131</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -3498,7 +3488,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C69" s="3">
         <v>816</v>
@@ -3509,7 +3499,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C70" s="3">
         <v>4</v>
@@ -3520,7 +3510,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C71" s="3">
         <v>4</v>
@@ -3531,7 +3521,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C72" s="3">
         <v>1</v>
@@ -3542,7 +3532,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C73" s="3">
         <v>3</v>
@@ -3553,7 +3543,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C74" s="3">
         <v>1</v>
@@ -3564,13 +3554,13 @@
         <v>73</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C75" s="3">
         <v>3</v>
       </c>
       <c r="D75" s="10">
-        <v>22618</v>
+        <v>2022618</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -3578,13 +3568,13 @@
         <v>74</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C76" s="3">
         <v>1</v>
       </c>
       <c r="D76" s="10">
-        <v>2019</v>
+        <v>202019</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -3592,13 +3582,13 @@
         <v>75</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C77" s="3">
         <v>2</v>
       </c>
       <c r="D77" s="10">
-        <v>21330</v>
+        <v>2021330</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -3606,7 +3596,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C78" s="3">
         <v>1</v>
@@ -3617,13 +3607,13 @@
         <v>77</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C79" s="3">
         <v>3</v>
       </c>
       <c r="D79" s="10">
-        <v>23121</v>
+        <v>2023121</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -3631,13 +3621,13 @@
         <v>78</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C80" s="3">
         <v>3</v>
       </c>
       <c r="D80" s="10">
-        <v>23514</v>
+        <v>2023514</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -3645,7 +3635,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C81" s="3">
         <v>3</v>
@@ -3656,7 +3646,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C82" s="3">
         <v>677</v>
@@ -3667,7 +3657,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C83" s="3">
         <v>2</v>
@@ -3678,7 +3668,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C84" s="3">
         <v>3</v>
@@ -3689,13 +3679,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C85" s="3">
         <v>2</v>
       </c>
       <c r="D85" s="10">
-        <v>20121</v>
+        <v>2020121</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -3703,7 +3693,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C86" s="3">
         <v>3</v>
@@ -3714,7 +3704,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C87" s="3">
         <v>1</v>
@@ -3725,13 +3715,13 @@
         <v>86</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C88" s="3">
         <v>2</v>
       </c>
       <c r="D88" s="10">
-        <v>20226</v>
+        <v>2020226</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
@@ -3739,13 +3729,13 @@
         <v>87</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C89" s="3">
         <v>1</v>
       </c>
       <c r="D89" s="10">
-        <v>25106</v>
+        <v>2025106</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
@@ -3753,7 +3743,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C90" s="3">
         <v>1</v>
@@ -3764,7 +3754,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C91" s="3">
         <v>2</v>
@@ -3775,13 +3765,13 @@
         <v>90</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C92" s="3">
         <v>4</v>
       </c>
       <c r="D92" s="10">
-        <v>21212</v>
+        <v>2021212</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
@@ -3789,13 +3779,13 @@
         <v>91</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C93" s="3">
         <v>3</v>
       </c>
       <c r="D93" s="10">
-        <v>22424</v>
+        <v>2022424</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -3803,7 +3793,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C94" s="3">
         <v>1151</v>
@@ -3814,7 +3804,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C95" s="3">
         <v>3</v>
@@ -3825,7 +3815,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C96" s="3">
         <v>642</v>
@@ -3836,13 +3826,13 @@
         <v>95</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C97" s="3">
         <v>1</v>
       </c>
       <c r="D97" s="10">
-        <v>21110</v>
+        <v>2021110</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
@@ -3850,7 +3840,7 @@
         <v>96</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C98" s="3">
         <v>485</v>
@@ -3861,7 +3851,7 @@
         <v>97</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C99" s="3">
         <v>2</v>
@@ -3872,7 +3862,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C100" s="3">
         <v>371</v>
@@ -3883,7 +3873,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C101" s="3">
         <v>3</v>
@@ -3894,10 +3884,24 @@
         <v>100</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C102" s="3">
         <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B103" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D103" s="10" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -3909,4 +3913,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:I10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="9" width="12.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="113" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="114"/>
+      <c r="D2" s="114"/>
+      <c r="E2" s="114"/>
+      <c r="F2" s="114"/>
+      <c r="G2" s="114"/>
+      <c r="H2" s="114"/>
+      <c r="I2" s="115"/>
+    </row>
+    <row r="3" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="117" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="118"/>
+      <c r="D3" s="118"/>
+      <c r="E3" s="119"/>
+      <c r="F3" s="117" t="s">
+        <v>100</v>
+      </c>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="119"/>
+    </row>
+    <row r="4" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="120"/>
+      <c r="C4" s="121"/>
+      <c r="D4" s="121"/>
+      <c r="E4" s="122"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="121"/>
+      <c r="I4" s="122"/>
+    </row>
+    <row r="5" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="116" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="108"/>
+      <c r="D5" s="108"/>
+      <c r="E5" s="109"/>
+      <c r="F5" s="107" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="108"/>
+      <c r="H5" s="108"/>
+      <c r="I5" s="109"/>
+    </row>
+    <row r="6" spans="2:9" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="110"/>
+      <c r="C6" s="111"/>
+      <c r="D6" s="111"/>
+      <c r="E6" s="112"/>
+      <c r="F6" s="110"/>
+      <c r="G6" s="111"/>
+      <c r="H6" s="111"/>
+      <c r="I6" s="112"/>
+    </row>
+    <row r="7" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:9" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="F5:I6"/>
+    <mergeCell ref="B2:I2"/>
+    <mergeCell ref="B5:E6"/>
+    <mergeCell ref="B3:E4"/>
+    <mergeCell ref="F3:I4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>